<commit_message>
Create Expense APIs 🖋️
</commit_message>
<xml_diff>
--- a/backend/income_details.xlsx
+++ b/backend/income_details.xlsx
@@ -1,44 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Expense_Tracker\backend\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{871F458D-26A6-47C7-94B9-1AE599ABDD0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="3732" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
     <sheet name="Income" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
-  <si>
-    <t>Source</t>
-  </si>
-  <si>
-    <t>Amount</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Salary</t>
-  </si>
-</sst>
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <numFmts count="1">
+    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+  </numFmts>
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -68,7 +65,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -76,14 +73,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -408,30 +397,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="3" max="3" width="9.5" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Source</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Amount</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Date</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Salary</v>
       </c>
       <c r="B2">
         <v>5600</v>
@@ -440,9 +425,9 @@
         <v>45728.229537037034</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>3</v>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Salary</v>
       </c>
       <c r="B3">
         <v>4600</v>
@@ -451,10 +436,31 @@
         <v>45728.229537037034</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Salary</v>
+      </c>
+      <c r="B4">
+        <v>4000</v>
+      </c>
+      <c r="C4" s="1">
+        <v>45728.229537037034</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Salary</v>
+      </c>
+      <c r="B5">
+        <v>5000</v>
+      </c>
+      <c r="C5" s="1">
+        <v>45728.229537037034</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:C3" numberStoredAsText="1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>